<commit_message>
Aplicado el tab para los condicionales
</commit_message>
<xml_diff>
--- a/proyecto_II_Prueba.xlsx
+++ b/proyecto_II_Prueba.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\Programación\Potencia 1\Proyecto_2_Ver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17089A2E-6A20-46AD-B9D5-58E813F47382}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CCB718E-74C6-4B05-90B9-58D3A3822600}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GEN" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="109">
   <si>
     <t>Tecnología de Generación</t>
   </si>
@@ -307,13 +307,7 @@
     <t xml:space="preserve">V Base </t>
   </si>
   <si>
-    <t>S base</t>
-  </si>
-  <si>
     <t>Z base</t>
-  </si>
-  <si>
-    <t>1,2,3,4</t>
   </si>
   <si>
     <t>Linea Barra 2-3</t>
@@ -340,7 +334,46 @@
     <t>7,8,9,10,13</t>
   </si>
   <si>
-    <t>Linea Barra 7-8</t>
+    <t>Linea Barra 9-10</t>
+  </si>
+  <si>
+    <t>Linea Barra 7-8/8-9</t>
+  </si>
+  <si>
+    <t>50 km a Bolivar</t>
+  </si>
+  <si>
+    <t>765 KV - 190 km</t>
+  </si>
+  <si>
+    <t>765 KV - 182 km</t>
+  </si>
+  <si>
+    <t>765 KV - 160 km</t>
+  </si>
+  <si>
+    <t>765 KV - 240 km</t>
+  </si>
+  <si>
+    <t>230KV - 240 km</t>
+  </si>
+  <si>
+    <t>Linea Barra 16-17</t>
+  </si>
+  <si>
+    <t>Linea Barra 10-13</t>
+  </si>
+  <si>
+    <t>Linea Barra 9-13</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>230KV - 220 km</t>
+  </si>
+  <si>
+    <t>Linea Barra 17-20</t>
   </si>
 </sst>
 </file>
@@ -430,7 +463,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -554,11 +587,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="hair">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="hair">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -713,12 +761,18 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="1" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="1" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2323,11 +2377,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AE1000"/>
   <sheetViews>
-    <sheetView zoomScale="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F15" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="70" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="G14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I27" sqref="I27:J27"/>
+      <selection pane="bottomRight" activeCell="I35" sqref="I35:K35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2336,7 +2390,8 @@
     <col min="2" max="2" width="19" customWidth="1"/>
     <col min="3" max="4" width="21.28515625" customWidth="1"/>
     <col min="5" max="6" width="16.7109375" customWidth="1"/>
-    <col min="7" max="8" width="43.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="34" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="43.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="38.42578125" customWidth="1"/>
     <col min="10" max="31" width="16.7109375" customWidth="1"/>
   </cols>
@@ -3348,22 +3403,16 @@
         <v>84</v>
       </c>
       <c r="B22" s="57" t="s">
+        <v>92</v>
+      </c>
+      <c r="C22" s="54" t="s">
+        <v>93</v>
+      </c>
+      <c r="D22" s="55" t="s">
+        <v>91</v>
+      </c>
+      <c r="E22" s="56" t="s">
         <v>94</v>
-      </c>
-      <c r="C22" s="54" t="s">
-        <v>95</v>
-      </c>
-      <c r="D22" s="55" t="s">
-        <v>93</v>
-      </c>
-      <c r="E22" s="56" t="s">
-        <v>96</v>
-      </c>
-      <c r="F22" t="s">
-        <v>84</v>
-      </c>
-      <c r="G22" t="s">
-        <v>88</v>
       </c>
       <c r="H22" s="63" t="s">
         <v>22</v>
@@ -3398,29 +3447,26 @@
         <f>765000</f>
         <v>765000</v>
       </c>
-      <c r="F23" t="s">
-        <v>85</v>
-      </c>
-      <c r="G23" s="34">
-        <v>400000</v>
-      </c>
-      <c r="H23" s="66"/>
-      <c r="I23" s="67">
+      <c r="G23" s="34"/>
+      <c r="H23" s="71" t="s">
+        <v>97</v>
+      </c>
+      <c r="I23" s="66">
         <f>I22/$B$25</f>
         <v>5.1468749999999995E-3</v>
       </c>
-      <c r="J23" s="67">
+      <c r="J23" s="66">
         <f>J22/$B$25</f>
         <v>6.7972500000000005E-2</v>
       </c>
-      <c r="K23" s="68">
+      <c r="K23" s="67">
         <f>K22/$B$25</f>
         <v>0.70556062499999994</v>
       </c>
     </row>
     <row r="24" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="52" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B24" s="50">
         <v>100000000</v>
@@ -3434,31 +3480,26 @@
       <c r="E24" s="34">
         <v>100000000</v>
       </c>
-      <c r="F24" t="s">
-        <v>86</v>
-      </c>
-      <c r="G24" s="34">
-        <v>100000000</v>
-      </c>
+      <c r="G24" s="34"/>
       <c r="H24" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="I24" s="69">
+      <c r="I24" s="68">
         <f>H5*$G$29</f>
         <v>2.7929999999999997</v>
       </c>
-      <c r="J24" s="69">
-        <f t="shared" ref="J24:K26" si="0">I5*$G$29</f>
+      <c r="J24" s="68">
+        <f t="shared" ref="J24:K24" si="0">I5*$G$29</f>
         <v>64.941999999999993</v>
       </c>
-      <c r="K24" s="70">
+      <c r="K24" s="69">
         <f t="shared" si="0"/>
         <v>927.56100000000004</v>
       </c>
     </row>
     <row r="25" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="45" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B25" s="53">
         <f>(B23*B23)/B24</f>
@@ -3476,39 +3517,35 @@
         <f>(E23*E23)/E24</f>
         <v>5852.25</v>
       </c>
-      <c r="F25" t="s">
-        <v>87</v>
-      </c>
-      <c r="G25" s="35">
-        <f>(G23*G23)/G24</f>
-        <v>1600</v>
-      </c>
-      <c r="H25" s="66"/>
-      <c r="I25" s="71">
+      <c r="G25" s="35"/>
+      <c r="H25" s="72" t="s">
+        <v>98</v>
+      </c>
+      <c r="I25" s="70">
         <f>I24/$E$25</f>
         <v>4.7725233884403427E-4</v>
       </c>
-      <c r="J25" s="71">
+      <c r="J25" s="70">
         <f t="shared" ref="J25:K25" si="1">J24/$E$25</f>
         <v>1.1096928531761287E-2</v>
       </c>
-      <c r="K25" s="68">
+      <c r="K25" s="67">
         <f t="shared" si="1"/>
         <v>0.15849647571446879</v>
       </c>
     </row>
     <row r="26" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G26" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="H26" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="I26" s="69">
+      <c r="I26" s="68">
         <f>H5*$G$30</f>
         <v>2.6753999999999998</v>
       </c>
-      <c r="J26" s="69">
+      <c r="J26" s="68">
         <f t="shared" ref="J26:K26" si="2">I5*$G$30</f>
         <v>62.207599999999999</v>
       </c>
@@ -3519,69 +3556,205 @@
     </row>
     <row r="27" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F27" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G27">
         <v>50</v>
       </c>
-      <c r="H27" s="66"/>
-      <c r="I27" s="71">
+      <c r="H27" s="72" t="s">
+        <v>99</v>
+      </c>
+      <c r="I27" s="70">
         <f>I26/$E$25</f>
         <v>4.571575035242855E-4</v>
       </c>
-      <c r="J27" s="71">
+      <c r="J27" s="70">
         <f t="shared" ref="J27:K27" si="3">J26/$E$25</f>
         <v>1.0629689435687128E-2</v>
       </c>
-      <c r="K27" s="71">
+      <c r="K27" s="67">
         <f t="shared" si="3"/>
         <v>0.15182293989491222</v>
       </c>
     </row>
     <row r="28" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F28" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G28" s="35">
         <v>270</v>
       </c>
-      <c r="H28" s="19"/>
-      <c r="I28" s="20"/>
+      <c r="H28" s="63" t="s">
+        <v>22</v>
+      </c>
+      <c r="I28" s="68">
+        <f>H5*$G$31</f>
+        <v>2.3519999999999999</v>
+      </c>
+      <c r="J28" s="68">
+        <f t="shared" ref="J28:K28" si="4">I5*$G$31</f>
+        <v>54.688000000000002</v>
+      </c>
+      <c r="K28" s="68">
+        <f t="shared" si="4"/>
+        <v>781.10400000000004</v>
+      </c>
     </row>
     <row r="29" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F29" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G29" s="19">
         <v>190</v>
       </c>
-      <c r="H29" s="20"/>
+      <c r="H29" s="72" t="s">
+        <v>100</v>
+      </c>
+      <c r="I29" s="70">
+        <f>I28/$E$25</f>
+        <v>4.0189670639497626E-4</v>
+      </c>
+      <c r="J29" s="70">
+        <f t="shared" ref="J29:K29" si="5">J28/$E$25</f>
+        <v>9.34478192148319E-3</v>
+      </c>
+      <c r="K29" s="67">
+        <f t="shared" si="5"/>
+        <v>0.13347071639113162</v>
+      </c>
     </row>
     <row r="30" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F30" t="s">
+        <v>95</v>
+      </c>
       <c r="G30" s="19">
         <v>182</v>
       </c>
-      <c r="H30" s="20"/>
+      <c r="H30" s="63" t="s">
+        <v>22</v>
+      </c>
+      <c r="I30" s="68">
+        <f>H5*$G$32</f>
+        <v>3.528</v>
+      </c>
+      <c r="J30" s="68">
+        <f t="shared" ref="J30:K30" si="6">I5*$G$32</f>
+        <v>82.031999999999996</v>
+      </c>
+      <c r="K30" s="68">
+        <f t="shared" si="6"/>
+        <v>1171.6559999999999</v>
+      </c>
     </row>
     <row r="31" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G31" s="19"/>
-      <c r="H31" s="20"/>
+      <c r="F31" t="s">
+        <v>105</v>
+      </c>
+      <c r="G31" s="19">
+        <v>160</v>
+      </c>
+      <c r="H31" s="72" t="s">
+        <v>101</v>
+      </c>
+      <c r="I31" s="70">
+        <f>I30/$E$25</f>
+        <v>6.0284505959246439E-4</v>
+      </c>
+      <c r="J31" s="70">
+        <f t="shared" ref="J31:K31" si="7">J30/$E$25</f>
+        <v>1.4017172882224784E-2</v>
+      </c>
+      <c r="K31" s="67">
+        <f t="shared" si="7"/>
+        <v>0.20020607458669742</v>
+      </c>
     </row>
     <row r="32" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G32" s="19"/>
-      <c r="H32" s="20"/>
+      <c r="F32" t="s">
+        <v>104</v>
+      </c>
+      <c r="G32" s="19">
+        <v>240</v>
+      </c>
+      <c r="H32" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="I32" s="73">
+        <f>H3*$G$33</f>
+        <v>17.928000000000001</v>
+      </c>
+      <c r="J32" s="73">
+        <f t="shared" ref="J32:K32" si="8">I3*$G$33</f>
+        <v>114.648</v>
+      </c>
+      <c r="K32" s="73">
+        <f t="shared" si="8"/>
+        <v>837.6</v>
+      </c>
     </row>
     <row r="33" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G33" s="19"/>
-      <c r="H33" s="20"/>
+      <c r="F33" t="s">
+        <v>103</v>
+      </c>
+      <c r="G33" s="19">
+        <v>240</v>
+      </c>
+      <c r="H33" s="74" t="s">
+        <v>102</v>
+      </c>
+      <c r="I33" s="75">
+        <f>I32/C25</f>
+        <v>3.3890359168241971E-2</v>
+      </c>
+      <c r="J33" s="75">
+        <f t="shared" ref="J33:K33" si="9">J32/D25</f>
+        <v>0.86690359168241959</v>
+      </c>
+      <c r="K33" s="75">
+        <f t="shared" si="9"/>
+        <v>0.14312443931821095</v>
+      </c>
     </row>
     <row r="34" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G34" s="19"/>
-      <c r="H34" s="20"/>
+      <c r="F34" t="s">
+        <v>108</v>
+      </c>
+      <c r="G34" s="19">
+        <v>220</v>
+      </c>
+      <c r="H34" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="I34">
+        <f>$G$34*H3</f>
+        <v>16.434000000000001</v>
+      </c>
+      <c r="J34">
+        <f t="shared" ref="J34:K34" si="10">$G$34*I3</f>
+        <v>105.09400000000001</v>
+      </c>
+      <c r="K34">
+        <f t="shared" si="10"/>
+        <v>767.80000000000007</v>
+      </c>
     </row>
     <row r="35" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G35" s="19"/>
-      <c r="H35" s="20"/>
+      <c r="H35" s="74" t="s">
+        <v>107</v>
+      </c>
+      <c r="I35">
+        <f>I34/$C$25</f>
+        <v>3.106616257088847E-2</v>
+      </c>
+      <c r="J35">
+        <f t="shared" ref="J35:K35" si="11">J34/$C$25</f>
+        <v>0.19866540642722119</v>
+      </c>
+      <c r="K35">
+        <f t="shared" si="11"/>
+        <v>1.4514177693761816</v>
+      </c>
     </row>
     <row r="36" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G36" s="19"/>
@@ -35356,7 +35529,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
@@ -35441,6 +35614,10 @@
         <f>I2*B2</f>
         <v>13.260266666666665</v>
       </c>
+      <c r="L2" s="60">
+        <f>J2/I20</f>
+        <v>2.5066666666666664E-2</v>
+      </c>
       <c r="M2" s="61">
         <f>J2/J20</f>
         <v>0.10026666666666666</v>
@@ -35483,6 +35660,10 @@
       <c r="L3" s="60">
         <f>J3/I20</f>
         <v>0.1462</v>
+      </c>
+      <c r="M3" s="61">
+        <f>J3/J20</f>
+        <v>0.58479999999999999</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -35872,16 +36053,16 @@
         <v>84</v>
       </c>
       <c r="H17" s="57" t="s">
+        <v>92</v>
+      </c>
+      <c r="I17" s="54" t="s">
+        <v>93</v>
+      </c>
+      <c r="J17" s="55" t="s">
+        <v>91</v>
+      </c>
+      <c r="K17" s="56" t="s">
         <v>94</v>
-      </c>
-      <c r="I17" s="54" t="s">
-        <v>95</v>
-      </c>
-      <c r="J17" s="55" t="s">
-        <v>93</v>
-      </c>
-      <c r="K17" s="56" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="18" spans="4:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -35910,7 +36091,7 @@
       <c r="E19" s="27"/>
       <c r="F19" s="27"/>
       <c r="G19" s="52" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="H19" s="50">
         <v>100000000</v>
@@ -35930,7 +36111,7 @@
       <c r="E20" s="27"/>
       <c r="F20" s="27"/>
       <c r="G20" s="45" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H20" s="53">
         <f>(H18*H18)/H19</f>
@@ -40867,7 +41048,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D2" sqref="D2"/>
+      <selection pane="bottomRight" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -41151,22 +41332,26 @@
     </row>
     <row r="10" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="11" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H12" t="s">
+        <v>106</v>
+      </c>
+    </row>
     <row r="13" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="45" t="s">
         <v>84</v>
       </c>
       <c r="C13" s="57" t="s">
+        <v>92</v>
+      </c>
+      <c r="D13" s="54" t="s">
+        <v>93</v>
+      </c>
+      <c r="E13" s="55" t="s">
+        <v>91</v>
+      </c>
+      <c r="F13" s="56" t="s">
         <v>94</v>
-      </c>
-      <c r="D13" s="54" t="s">
-        <v>95</v>
-      </c>
-      <c r="E13" s="55" t="s">
-        <v>93</v>
-      </c>
-      <c r="F13" s="56" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -41189,7 +41374,7 @@
     </row>
     <row r="15" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="52" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C15" s="50">
         <v>100000000</v>
@@ -41206,7 +41391,7 @@
     </row>
     <row r="16" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="45" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C16" s="53">
         <f>(C14*C14)/C15</f>

</xml_diff>

<commit_message>
Terminado el sistema de proyecto
</commit_message>
<xml_diff>
--- a/proyecto_II_Prueba.xlsx
+++ b/proyecto_II_Prueba.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\Programación\Potencia 1\Proyecto_2_Ver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CCB718E-74C6-4B05-90B9-58D3A3822600}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9DBE6A2-5FCF-4EE8-B364-4B3D51D266EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GEN" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="115">
   <si>
     <t>Tecnología de Generación</t>
   </si>
@@ -375,6 +375,24 @@
   <si>
     <t>Linea Barra 17-20</t>
   </si>
+  <si>
+    <t>230KV - 135 km</t>
+  </si>
+  <si>
+    <t>Linea Barra 23-24</t>
+  </si>
+  <si>
+    <t>Linea Barra 20-21</t>
+  </si>
+  <si>
+    <t>400 KV - 138 km</t>
+  </si>
+  <si>
+    <t>Linea Barra 20-25</t>
+  </si>
+  <si>
+    <t>230KV - 230 km</t>
+  </si>
 </sst>
 </file>
 
@@ -606,7 +624,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -773,6 +791,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2377,11 +2396,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AE1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="G14" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="70" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I35" sqref="I35:K35"/>
+      <selection pane="bottomRight" activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3739,7 +3758,12 @@
       </c>
     </row>
     <row r="35" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G35" s="19"/>
+      <c r="F35" t="s">
+        <v>111</v>
+      </c>
+      <c r="G35" s="19">
+        <v>135</v>
+      </c>
       <c r="H35" s="74" t="s">
         <v>107</v>
       </c>
@@ -3757,16 +3781,68 @@
       </c>
     </row>
     <row r="36" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G36" s="19"/>
-      <c r="H36" s="20"/>
+      <c r="F36" t="s">
+        <v>110</v>
+      </c>
+      <c r="G36" s="19">
+        <v>138</v>
+      </c>
+      <c r="H36" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="I36">
+        <f>$G$35*H3</f>
+        <v>10.0845</v>
+      </c>
+      <c r="J36">
+        <f t="shared" ref="J36:K36" si="12">$G$35*I3</f>
+        <v>64.489500000000007</v>
+      </c>
+      <c r="K36">
+        <f t="shared" si="12"/>
+        <v>471.15000000000003</v>
+      </c>
     </row>
     <row r="37" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G37" s="19"/>
-      <c r="H37" s="20"/>
+      <c r="F37" t="s">
+        <v>113</v>
+      </c>
+      <c r="G37" s="19">
+        <v>230</v>
+      </c>
+      <c r="H37" s="74" t="s">
+        <v>109</v>
+      </c>
+      <c r="I37">
+        <f>I36/$C$25</f>
+        <v>1.9063327032136108E-2</v>
+      </c>
+      <c r="J37">
+        <f t="shared" ref="J37:K37" si="13">J36/$C$25</f>
+        <v>0.12190831758034028</v>
+      </c>
+      <c r="K37">
+        <f t="shared" si="13"/>
+        <v>0.8906427221172023</v>
+      </c>
     </row>
     <row r="38" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G38" s="19"/>
-      <c r="H38" s="20"/>
+      <c r="H38" s="63" t="s">
+        <v>22</v>
+      </c>
+      <c r="I38" s="64">
+        <f>H4*$G$36</f>
+        <v>4.2089999999999996</v>
+      </c>
+      <c r="J38" s="64">
+        <f t="shared" ref="J38:K38" si="14">I4*$G$36</f>
+        <v>55.586399999999998</v>
+      </c>
+      <c r="K38" s="64">
+        <f t="shared" si="14"/>
+        <v>576.99180000000001</v>
+      </c>
     </row>
     <row r="39" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="16"/>
@@ -3776,10 +3852,21 @@
       <c r="E39" s="16"/>
       <c r="F39" s="16"/>
       <c r="G39" s="21"/>
-      <c r="H39" s="22"/>
-      <c r="I39" s="16"/>
-      <c r="J39" s="22"/>
-      <c r="K39" s="23"/>
+      <c r="H39" s="71" t="s">
+        <v>112</v>
+      </c>
+      <c r="I39" s="66">
+        <f>I38/$B$25</f>
+        <v>2.6306249999999997E-3</v>
+      </c>
+      <c r="J39" s="66">
+        <f>J38/$B$25</f>
+        <v>3.4741500000000002E-2</v>
+      </c>
+      <c r="K39" s="67">
+        <f>K38/$B$25</f>
+        <v>0.36061987500000003</v>
+      </c>
       <c r="L39" s="16"/>
       <c r="M39" s="16"/>
       <c r="N39" s="16"/>
@@ -3809,10 +3896,21 @@
       <c r="E40" s="16"/>
       <c r="F40" s="16"/>
       <c r="G40" s="21"/>
-      <c r="H40" s="22"/>
-      <c r="I40" s="16"/>
-      <c r="J40" s="22"/>
-      <c r="K40" s="23"/>
+      <c r="H40" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="I40" s="73">
+        <f>H3*$G$37</f>
+        <v>17.181000000000001</v>
+      </c>
+      <c r="J40" s="73">
+        <f t="shared" ref="J40:K40" si="15">I3*$G$37</f>
+        <v>109.87100000000001</v>
+      </c>
+      <c r="K40" s="73">
+        <f t="shared" si="15"/>
+        <v>802.7</v>
+      </c>
       <c r="L40" s="16"/>
       <c r="M40" s="16"/>
       <c r="N40" s="16"/>
@@ -3842,10 +3940,21 @@
       <c r="E41" s="16"/>
       <c r="F41" s="16"/>
       <c r="G41" s="21"/>
-      <c r="H41" s="22"/>
-      <c r="I41" s="16"/>
-      <c r="J41" s="22"/>
-      <c r="K41" s="23"/>
+      <c r="H41" s="74" t="s">
+        <v>114</v>
+      </c>
+      <c r="I41" s="75">
+        <f>I40/$C$25</f>
+        <v>3.247826086956522E-2</v>
+      </c>
+      <c r="J41" s="75">
+        <f t="shared" ref="J41:K41" si="16">J40/$C$25</f>
+        <v>0.20769565217391306</v>
+      </c>
+      <c r="K41" s="75">
+        <f t="shared" si="16"/>
+        <v>1.5173913043478262</v>
+      </c>
       <c r="L41" s="16"/>
       <c r="M41" s="16"/>
       <c r="N41" s="16"/>
@@ -35530,7 +35639,7 @@
   <dimension ref="A1:N1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -35838,6 +35947,10 @@
         <f t="shared" si="1"/>
         <v>53.12</v>
       </c>
+      <c r="K8" s="76">
+        <f>J8/H20</f>
+        <v>3.32E-2</v>
+      </c>
       <c r="L8" s="60">
         <f>J8/I20</f>
         <v>0.10041587901701322</v>
@@ -41048,7 +41161,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D5" sqref="D5"/>
+      <selection pane="bottomRight" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -42408,7 +42521,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>